<commit_message>
mod: fit symbol to firstline length
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishii\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ishii\work\deno\XlsxToMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE533CBA-4D00-4149-B601-B73F310F1590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADE2A76-37DC-438A-A379-640B78D5E518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0E4BDDC0-95DA-4F21-9C32-6DD91076B93A}"/>
   </bookViews>
@@ -38,29 +38,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>a</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>b</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>f</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sample1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>long name test pattern</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>long long test</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -99,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,41 +126,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -164,12 +140,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -489,53 +459,53 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2">
-        <v>3</v>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3">
-        <v>31</v>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>